<commit_message>
Moved 'smoker' comp to dataprep
</commit_message>
<xml_diff>
--- a/Output/DescriptiveClinical.xlsx
+++ b/Output/DescriptiveClinical.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -378,6 +378,21 @@
           <t>PG (29)</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>HCn</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Gn</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>PGn</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -400,6 +415,21 @@
           <t>26.66 (6.4) | 24</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NotOk</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -444,6 +474,21 @@
           <t>14.31 (2.12) | 15</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -466,6 +511,16 @@
           <t>10.24 (5.64) | 8</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -488,6 +543,21 @@
           <t>8.81 (7.42) | 7</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -510,6 +580,21 @@
           <t>12.25 (7.89) | 9</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -532,6 +617,21 @@
           <t>2.71 (2.69) | 2</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -576,6 +676,21 @@
           <t>16.97 (7.6) | 17</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -598,6 +713,21 @@
           <t>31.45 (8.59) | 32</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -620,6 +750,21 @@
           <t>48.83 (8.04) | 47</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -642,6 +787,21 @@
           <t>10.24 (2.59) | 10</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -664,6 +824,21 @@
           <t>11.21 (2.21) | 12</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -686,6 +861,21 @@
           <t>7.79 (2.4) | 8</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>NotOk</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -708,6 +898,21 @@
           <t>7.48 (2.64) | 7</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -730,6 +935,21 @@
           <t>12.1 (2.04) | 12</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -752,6 +972,21 @@
           <t>34.31 (5.95) | 35</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -774,6 +1009,21 @@
           <t>25.55 (9.52) | 26</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>NotOk</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -796,6 +1046,21 @@
           <t>6.48 (5.38) | 5</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -818,6 +1083,21 @@
           <t>65.14 (14.47) | 62</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -838,6 +1118,21 @@
       <c r="D22" t="inlineStr">
         <is>
           <t>42.28 (11.29) | 41</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>

</xml_diff>